<commit_message>
fixed diet absob effi bug
</commit_message>
<xml_diff>
--- a/tests/Arnot_match_Sediment_Total_Water.xlsx
+++ b/tests/Arnot_match_Sediment_Total_Water.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sample and Time Input" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="120">
   <si>
     <t xml:space="preserve">Sampling Variables Inputs</t>
   </si>
@@ -318,6 +318,9 @@
     <t xml:space="preserve">Filter Feeder Flag (0 = is, and 1 = is not)</t>
   </si>
   <si>
+    <t xml:space="preserve">Small White Sucker</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gammarus</t>
   </si>
   <si>
@@ -418,7 +421,7 @@
     <numFmt numFmtId="166" formatCode="M/D/YYYY"/>
     <numFmt numFmtId="167" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="25">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -558,6 +561,20 @@
     </font>
     <font>
       <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
@@ -800,7 +817,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="74">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1033,6 +1050,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="23" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1042,6 +1063,26 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="15" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="15" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1156,9 +1197,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1018080</xdr:colOff>
+      <xdr:colOff>1017720</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>188640</xdr:rowOff>
+      <xdr:rowOff>188280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1168,7 +1209,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="14044680" y="863280"/>
-          <a:ext cx="9470520" cy="7618320"/>
+          <a:ext cx="9470160" cy="7617960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1635,9 +1676,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>3630240</xdr:colOff>
+      <xdr:colOff>3629880</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>181800</xdr:rowOff>
+      <xdr:rowOff>181440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1647,7 +1688,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12356640" y="699480"/>
-          <a:ext cx="3083760" cy="994680"/>
+          <a:ext cx="3083400" cy="994320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1858,9 +1899,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2330640</xdr:colOff>
+      <xdr:colOff>2330280</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>188640</xdr:rowOff>
+      <xdr:rowOff>188280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1874,7 +1915,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16507800" y="10278720"/>
-          <a:ext cx="2330640" cy="734760"/>
+          <a:ext cx="2330280" cy="734400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1895,7 +1936,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>4759920</xdr:colOff>
+      <xdr:colOff>4759560</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>87120</xdr:rowOff>
     </xdr:to>
@@ -1907,7 +1948,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11824920" y="2007000"/>
-          <a:ext cx="9442800" cy="3200760"/>
+          <a:ext cx="9442440" cy="3200760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2374,9 +2415,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>255240</xdr:colOff>
+      <xdr:colOff>254880</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>141480</xdr:rowOff>
+      <xdr:rowOff>141120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2386,7 +2427,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16398360" y="1476360"/>
-          <a:ext cx="3602520" cy="760320"/>
+          <a:ext cx="3602160" cy="759960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2516,9 +2557,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1132200</xdr:colOff>
+      <xdr:colOff>1131840</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>188640</xdr:rowOff>
+      <xdr:rowOff>188280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2528,7 +2569,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="14774760" y="1714680"/>
-          <a:ext cx="2930040" cy="759960"/>
+          <a:ext cx="2929680" cy="759600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3275,9 +3316,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>642600</xdr:colOff>
+      <xdr:colOff>642240</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>131760</xdr:rowOff>
+      <xdr:rowOff>131400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3287,7 +3328,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8870760" y="2521800"/>
-          <a:ext cx="9087480" cy="3567240"/>
+          <a:ext cx="9087120" cy="3566880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3815,9 +3856,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>150480</xdr:colOff>
+      <xdr:colOff>150120</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>9360</xdr:rowOff>
+      <xdr:rowOff>9000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3827,7 +3868,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8939880" y="674280"/>
-          <a:ext cx="4074840" cy="948600"/>
+          <a:ext cx="4074480" cy="948240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3928,15 +3969,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>4629240</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>47160</xdr:rowOff>
+      <xdr:colOff>3687120</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>121320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>3565800</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:colOff>2623320</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>119160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3945,8 +3986,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4629240" y="4925160"/>
-          <a:ext cx="5157360" cy="760320"/>
+          <a:off x="3687120" y="6713640"/>
+          <a:ext cx="5157000" cy="759960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4048,9 +4089,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2592360</xdr:colOff>
+      <xdr:colOff>2592000</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>189360</xdr:rowOff>
+      <xdr:rowOff>189000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4060,7 +4101,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16049880" y="5488560"/>
-          <a:ext cx="4330440" cy="340560"/>
+          <a:ext cx="4330080" cy="340200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4132,9 +4173,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>5383080</xdr:colOff>
+      <xdr:colOff>5382720</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>137880</xdr:rowOff>
+      <xdr:rowOff>137520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4144,7 +4185,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9213840" y="76320"/>
-          <a:ext cx="5256000" cy="1496520"/>
+          <a:ext cx="5255640" cy="1496160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4206,14 +4247,14 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>274320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>825480</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>10080</xdr:rowOff>
+      <xdr:rowOff>4680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4252,13 +4293,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>825480</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>10080</xdr:rowOff>
+      <xdr:rowOff>4680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>825840</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>139680</xdr:rowOff>
+      <xdr:rowOff>133920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4297,13 +4338,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>139680</xdr:rowOff>
+      <xdr:rowOff>133920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>825480</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>140040</xdr:rowOff>
+      <xdr:rowOff>134280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4346,7 +4387,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>6883560</xdr:colOff>
+      <xdr:colOff>6883200</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>87120</xdr:rowOff>
     </xdr:to>
@@ -4357,8 +4398,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10153440" y="2298600"/>
-          <a:ext cx="5816880" cy="658440"/>
+          <a:off x="10153440" y="2304360"/>
+          <a:ext cx="5816520" cy="658440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4465,9 +4506,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>252360</xdr:colOff>
+      <xdr:colOff>252000</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>61560</xdr:rowOff>
+      <xdr:rowOff>61200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4477,7 +4518,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11960640" y="241200"/>
-          <a:ext cx="5135400" cy="391680"/>
+          <a:ext cx="5135040" cy="391320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4589,9 +4630,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>99720</xdr:colOff>
+      <xdr:colOff>99360</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>188640</xdr:rowOff>
+      <xdr:rowOff>188280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4601,7 +4642,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12062160" y="1295280"/>
-          <a:ext cx="3861720" cy="417240"/>
+          <a:ext cx="3861360" cy="416880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4658,9 +4699,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>468360</xdr:colOff>
+      <xdr:colOff>468000</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>188640</xdr:rowOff>
+      <xdr:rowOff>188280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4670,7 +4711,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12087720" y="2158560"/>
-          <a:ext cx="5224320" cy="696960"/>
+          <a:ext cx="5223960" cy="696600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4727,9 +4768,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>644400</xdr:colOff>
+      <xdr:colOff>644040</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>61560</xdr:rowOff>
+      <xdr:rowOff>61200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4739,7 +4780,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="36809280" y="241200"/>
-          <a:ext cx="4103640" cy="391680"/>
+          <a:ext cx="4103280" cy="391320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4806,9 +4847,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>55</xdr:col>
-      <xdr:colOff>949320</xdr:colOff>
+      <xdr:colOff>948960</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>61560</xdr:rowOff>
+      <xdr:rowOff>61200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4818,7 +4859,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="59091120" y="241200"/>
-          <a:ext cx="4562280" cy="391680"/>
+          <a:ext cx="4561920" cy="391320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4885,9 +4926,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>76</xdr:col>
-      <xdr:colOff>691200</xdr:colOff>
+      <xdr:colOff>690840</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>61560</xdr:rowOff>
+      <xdr:rowOff>61200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4897,7 +4938,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="81165600" y="241200"/>
-          <a:ext cx="3645720" cy="391680"/>
+          <a:ext cx="3645360" cy="391320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4964,9 +5005,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>97</xdr:col>
-      <xdr:colOff>948960</xdr:colOff>
+      <xdr:colOff>948600</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>61560</xdr:rowOff>
+      <xdr:rowOff>61200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4976,7 +5017,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="101922840" y="241200"/>
-          <a:ext cx="4562280" cy="391680"/>
+          <a:ext cx="4561920" cy="391320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5043,9 +5084,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>118</xdr:col>
-      <xdr:colOff>691200</xdr:colOff>
+      <xdr:colOff>690840</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>61560</xdr:rowOff>
+      <xdr:rowOff>61200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5055,7 +5096,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="123997680" y="241200"/>
-          <a:ext cx="3645720" cy="391680"/>
+          <a:ext cx="3645360" cy="391320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5127,9 +5168,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>277560</xdr:colOff>
+      <xdr:colOff>277200</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>163440</xdr:rowOff>
+      <xdr:rowOff>163080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5139,7 +5180,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="13899240" y="761760"/>
-          <a:ext cx="6530040" cy="5878440"/>
+          <a:ext cx="6529680" cy="5878080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7749,8 +7790,8 @@
   </sheetPr>
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7999,9 +8040,11 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="23" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2"/>
-      <c r="B13" s="17" t="s">
-        <v>62</v>
+      <c r="A13" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="44" t="s">
+        <v>51</v>
       </c>
       <c r="C13" s="44" t="s">
         <v>69</v>
@@ -8015,18 +8058,26 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
+      <c r="A14" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="46" t="s">
+        <v>89</v>
+      </c>
       <c r="C14" s="27" t="s">
         <v>17</v>
       </c>
       <c r="D14" s="47" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
+      <c r="A15" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="58" t="n">
+        <v>0.029</v>
+      </c>
       <c r="C15" s="27" t="s">
         <v>74</v>
       </c>
@@ -8035,8 +8086,12 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
+      <c r="A16" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" s="12" t="n">
+        <v>0.055</v>
+      </c>
       <c r="C16" s="27" t="s">
         <v>76</v>
       </c>
@@ -8045,16 +8100,20 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
+      <c r="A17" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="12"/>
       <c r="C17" s="27" t="s">
         <v>78</v>
       </c>
       <c r="D17" s="47"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3"/>
-      <c r="B18" s="17"/>
+      <c r="A18" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="16"/>
       <c r="C18" s="27" t="s">
         <v>80</v>
       </c>
@@ -8063,48 +8122,62 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3"/>
-      <c r="B19" s="17"/>
+      <c r="A19" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="50"/>
       <c r="C19" s="27" t="s">
         <v>82</v>
       </c>
       <c r="D19" s="12"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3"/>
-      <c r="B20" s="17"/>
+      <c r="A20" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="B20" s="50"/>
       <c r="C20" s="27" t="s">
         <v>84</v>
       </c>
       <c r="D20" s="12"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
+      <c r="A21" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" s="47"/>
       <c r="C21" s="27" t="s">
         <v>86</v>
       </c>
       <c r="D21" s="12"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
+      <c r="A22" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" s="52"/>
       <c r="C22" s="1" t="s">
         <v>87</v>
       </c>
       <c r="D22" s="12"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
+      <c r="A23" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" s="47"/>
       <c r="C23" s="1" t="s">
         <v>75</v>
       </c>
       <c r="D23" s="53"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
+      <c r="A24" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="53" t="n">
+        <v>0</v>
+      </c>
       <c r="C24" s="54" t="s">
         <v>88</v>
       </c>
@@ -8113,6 +8186,9 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0" t="s">
+        <v>62</v>
+      </c>
       <c r="D25" s="0" t="s">
         <v>62</v>
       </c>
@@ -8136,8 +8212,8 @@
   </sheetPr>
   <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8149,56 +8225,56 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="60" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="61" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="61"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="61" t="n">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="61" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="61" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="61" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="61" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="61" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="61" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="61" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="60" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" s="60"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="60" t="s">
-        <v>91</v>
-      </c>
-      <c r="B3" s="60" t="n">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="60" t="s">
-        <v>71</v>
-      </c>
-      <c r="B4" s="60" t="n">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="60" t="s">
-        <v>70</v>
-      </c>
-      <c r="B5" s="60" t="n">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="60" t="s">
-        <v>73</v>
-      </c>
-      <c r="B6" s="60" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="B7" s="60" t="n">
+      <c r="B7" s="61" t="n">
         <v>0</v>
       </c>
       <c r="C7" s="31"/>
@@ -8206,156 +8282,299 @@
       <c r="E7" s="31"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="60" t="s">
+      <c r="A8" s="61" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="60" t="n">
+      <c r="B8" s="61" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="23" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="58" t="s">
+    <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="63" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="59" t="s">
+      <c r="B10" s="60" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="61" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="B10" s="60"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="60" t="s">
-        <v>91</v>
-      </c>
-      <c r="B11" s="60" t="n">
+      <c r="B11" s="61"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" s="61" t="n">
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="60" t="s">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="60" t="n">
+      <c r="B13" s="61" t="n">
         <v>0.1</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="60" t="s">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="61" t="s">
         <v>70</v>
       </c>
-      <c r="B13" s="60" t="n">
+      <c r="B14" s="61" t="n">
         <v>0.4</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="60" t="s">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="61" t="s">
         <v>73</v>
       </c>
-      <c r="B14" s="60" t="n">
+      <c r="B15" s="61" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="B15" s="60" t="n">
-        <v>0</v>
-      </c>
-    </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="60" t="s">
-        <v>72</v>
-      </c>
-      <c r="B16" s="60" t="n">
+      <c r="A16" s="61" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16" s="61" t="n">
         <v>0</v>
       </c>
       <c r="H16" s="31"/>
       <c r="I16" s="31"/>
       <c r="J16" s="31"/>
     </row>
-    <row r="17" customFormat="false" ht="23" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="58" t="s">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="61" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="63" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="59" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="60" t="s">
+      <c r="B19" s="60" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="61" t="s">
         <v>72</v>
       </c>
-      <c r="B18" s="60"/>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="60" t="s">
-        <v>91</v>
-      </c>
-      <c r="B19" s="60" t="n">
+      <c r="B20" s="61"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" s="61" t="n">
         <v>0.05</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="60" t="s">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="B20" s="60" t="n">
+      <c r="B22" s="61" t="n">
         <v>0.15</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="60" t="s">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="61" t="s">
         <v>70</v>
       </c>
-      <c r="B21" s="60" t="n">
+      <c r="B23" s="61" t="n">
         <v>0.7</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="60" t="s">
-        <v>73</v>
-      </c>
-      <c r="B22" s="60" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="B23" s="60" t="n">
-        <v>0.1</v>
       </c>
       <c r="H23" s="31"/>
       <c r="I23" s="31"/>
       <c r="J23" s="31"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="60" t="s">
+      <c r="A24" s="61" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" s="31"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="61" t="s">
+        <v>90</v>
+      </c>
+      <c r="B25" s="61" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="61" t="s">
         <v>72</v>
       </c>
-      <c r="B24" s="60" t="n">
+      <c r="B26" s="61" t="n">
         <v>0</v>
       </c>
-      <c r="H24" s="31"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="B27" s="63" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="60" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="61" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" s="61"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="B30" s="61" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="61" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" s="61" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="61" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" s="61" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="61" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" s="61" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="61" t="s">
+        <v>90</v>
+      </c>
+      <c r="B34" s="61" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" s="61" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="B36" s="63" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="64"/>
+      <c r="B37" s="64"/>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="64"/>
+      <c r="B38" s="64"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="31"/>
-      <c r="B39" s="31"/>
+      <c r="A39" s="64"/>
+      <c r="B39" s="64"/>
       <c r="C39" s="31"/>
     </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="64"/>
+      <c r="B40" s="64"/>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="64"/>
+      <c r="B41" s="64"/>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="64"/>
+      <c r="B42" s="64"/>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="64"/>
+      <c r="B43" s="64"/>
+    </row>
+    <row r="44" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="65"/>
+      <c r="B44" s="66"/>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="64"/>
+      <c r="B45" s="64"/>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="64"/>
+      <c r="B46" s="64"/>
+    </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="31"/>
-      <c r="B47" s="31"/>
+      <c r="A47" s="64"/>
+      <c r="B47" s="64"/>
       <c r="C47" s="31"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="31"/>
+      <c r="A48" s="64"/>
+      <c r="B48" s="64"/>
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="64"/>
+      <c r="B49" s="64"/>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="64"/>
+      <c r="B50" s="64"/>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="64"/>
+      <c r="B51" s="64"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="31"/>
@@ -8413,13 +8632,13 @@
         <v>68</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E1" s="17"/>
       <c r="TU1" s="0"/>
@@ -8908,385 +9127,385 @@
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="67" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="I2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="K2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="L2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="M2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="N2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="O2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="P2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="R2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="S2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="T2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="U2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="V2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="W2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="X2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="AF2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="AG2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="AS2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="AW2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="AY2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="AZ2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="BA2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="BB2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="BC2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="BD2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="BE2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="BF2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="BG2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="BH2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="BI2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="BJ2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="BK2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="BL2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="BM2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="BN2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="BO2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="BP2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="BQ2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="BR2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="BS2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="BT2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="BU2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="BV2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="BW2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="BX2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="BY2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="BZ2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="CA2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="CB2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="CC2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="CD2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="CE2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="CF2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="CG2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="CH2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="CI2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="CJ2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="CK2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="CL2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="CM2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="CN2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="CO2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="CP2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="CQ2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="CR2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="CS2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="CT2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="CU2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="CV2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="CW2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="CX2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="CY2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="CZ2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="DA2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="DB2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="DC2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="DD2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="DE2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="DF2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="DG2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="DH2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="DI2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="DJ2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="DK2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="DL2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="DM2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="DN2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="DO2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="DP2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="DQ2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="DR2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="DS2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="DT2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="DU2" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="DV2" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="DW2" s="63" t="n">
+      <c r="B2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="N2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="P2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="R2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="S2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="T2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="U2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="V2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="W2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="X2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="AU2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="AW2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="AY2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="AZ2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="BA2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="BC2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="BD2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="BE2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="BF2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="BG2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="BH2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="BI2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="BJ2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="BK2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="BL2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="BM2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="BN2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="BP2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="BQ2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="BR2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="BS2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="BT2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="BU2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="BV2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="BW2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="BX2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="BY2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="BZ2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="CB2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="CC2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="CD2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="CE2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="CF2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="CG2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="CH2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="CI2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="CJ2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="CK2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="CL2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="CM2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="CN2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="CO2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="CP2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="CQ2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="CR2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="CS2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="CT2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="CU2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="CV2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="CW2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="CX2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="CY2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="CZ2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="DA2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="DB2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="DC2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="DD2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="DE2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="DF2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="DG2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="DH2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="DI2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="DJ2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="DK2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="DL2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="DM2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="DN2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="DO2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="DP2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="DQ2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="DR2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="DS2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="DT2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="DU2" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="DV2" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="DW2" s="69" t="n">
         <v>1</v>
       </c>
       <c r="FU2" s="31"/>
@@ -9345,19 +9564,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F1" s="31"/>
       <c r="G1" s="31"/>
@@ -9366,16 +9585,16 @@
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="12"/>
       <c r="B2" s="12" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F2" s="31"/>
       <c r="G2" s="31"/>
@@ -9383,13 +9602,13 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D3" s="31"/>
       <c r="E3" s="31"/>
@@ -9403,7 +9622,7 @@
         <v>18</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D4" s="31"/>
       <c r="E4" s="31"/>
@@ -9742,9 +9961,9 @@
       <c r="H37" s="31"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="64"/>
-      <c r="B38" s="64"/>
-      <c r="C38" s="64"/>
+      <c r="A38" s="70"/>
+      <c r="B38" s="70"/>
+      <c r="C38" s="70"/>
       <c r="D38" s="31"/>
       <c r="E38" s="31"/>
       <c r="F38" s="31"/>
@@ -9752,17 +9971,17 @@
       <c r="H38" s="31"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="65" t="s">
-        <v>108</v>
-      </c>
-      <c r="B39" s="65" t="n">
+      <c r="A39" s="71" t="s">
+        <v>109</v>
+      </c>
+      <c r="B39" s="71" t="n">
         <v>40</v>
       </c>
-      <c r="C39" s="65" t="s">
-        <v>109</v>
-      </c>
-      <c r="D39" s="65" t="s">
+      <c r="C39" s="71" t="s">
         <v>110</v>
+      </c>
+      <c r="D39" s="71" t="s">
+        <v>111</v>
       </c>
       <c r="E39" s="31"/>
       <c r="F39" s="31"/>
@@ -9770,50 +9989,50 @@
       <c r="H39" s="31"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="62" t="s">
-        <v>111</v>
-      </c>
-      <c r="B40" s="62" t="s">
+      <c r="A40" s="68" t="s">
         <v>112</v>
       </c>
-      <c r="C40" s="62" t="s">
+      <c r="B40" s="68" t="s">
         <v>113</v>
       </c>
-      <c r="D40" s="66" t="s">
+      <c r="C40" s="68" t="s">
         <v>114</v>
       </c>
-      <c r="E40" s="66" t="s">
+      <c r="D40" s="72" t="s">
         <v>115</v>
       </c>
-      <c r="F40" s="66" t="s">
+      <c r="E40" s="72" t="s">
         <v>116</v>
       </c>
-      <c r="G40" s="66" t="s">
+      <c r="F40" s="72" t="s">
         <v>117</v>
       </c>
-      <c r="H40" s="67"/>
+      <c r="G40" s="72" t="s">
+        <v>118</v>
+      </c>
+      <c r="H40" s="73"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="62" t="s">
-        <v>118</v>
-      </c>
-      <c r="B41" s="62" t="s">
+      <c r="A41" s="68" t="s">
+        <v>119</v>
+      </c>
+      <c r="B41" s="68" t="s">
         <v>72</v>
       </c>
-      <c r="C41" s="62" t="n">
+      <c r="C41" s="68" t="n">
         <v>1</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F41" s="12" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G41" s="12" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H41" s="31"/>
       <c r="AW41" s="0" t="s">
@@ -9821,182 +10040,182 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="62"/>
-      <c r="B42" s="63"/>
-      <c r="C42" s="62"/>
-      <c r="D42" s="62"/>
-      <c r="E42" s="62"/>
-      <c r="F42" s="62"/>
-      <c r="G42" s="62"/>
+      <c r="A42" s="68"/>
+      <c r="B42" s="69"/>
+      <c r="C42" s="68"/>
+      <c r="D42" s="68"/>
+      <c r="E42" s="68"/>
+      <c r="F42" s="68"/>
+      <c r="G42" s="68"/>
       <c r="H42" s="31"/>
       <c r="AW42" s="0" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="63"/>
-      <c r="B43" s="63"/>
-      <c r="C43" s="63"/>
-      <c r="D43" s="63"/>
-      <c r="E43" s="63"/>
-      <c r="F43" s="63"/>
-      <c r="G43" s="63"/>
+      <c r="A43" s="69"/>
+      <c r="B43" s="69"/>
+      <c r="C43" s="69"/>
+      <c r="D43" s="69"/>
+      <c r="E43" s="69"/>
+      <c r="F43" s="69"/>
+      <c r="G43" s="69"/>
       <c r="AW43" s="0" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="63"/>
-      <c r="B44" s="63"/>
-      <c r="C44" s="63"/>
-      <c r="D44" s="63"/>
-      <c r="E44" s="63"/>
-      <c r="F44" s="63"/>
-      <c r="G44" s="63"/>
+      <c r="A44" s="69"/>
+      <c r="B44" s="69"/>
+      <c r="C44" s="69"/>
+      <c r="D44" s="69"/>
+      <c r="E44" s="69"/>
+      <c r="F44" s="69"/>
+      <c r="G44" s="69"/>
       <c r="AW44" s="0" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="63"/>
-      <c r="B45" s="63"/>
-      <c r="C45" s="63"/>
-      <c r="D45" s="63"/>
-      <c r="E45" s="63"/>
-      <c r="F45" s="63"/>
-      <c r="G45" s="63"/>
+      <c r="A45" s="69"/>
+      <c r="B45" s="69"/>
+      <c r="C45" s="69"/>
+      <c r="D45" s="69"/>
+      <c r="E45" s="69"/>
+      <c r="F45" s="69"/>
+      <c r="G45" s="69"/>
       <c r="AW45" s="0" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="63"/>
-      <c r="B46" s="63"/>
-      <c r="C46" s="63"/>
-      <c r="D46" s="63"/>
-      <c r="E46" s="63"/>
-      <c r="F46" s="63"/>
-      <c r="G46" s="63"/>
+      <c r="A46" s="69"/>
+      <c r="B46" s="69"/>
+      <c r="C46" s="69"/>
+      <c r="D46" s="69"/>
+      <c r="E46" s="69"/>
+      <c r="F46" s="69"/>
+      <c r="G46" s="69"/>
       <c r="AW46" s="0" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="63"/>
-      <c r="B47" s="63"/>
-      <c r="C47" s="63"/>
-      <c r="D47" s="63"/>
-      <c r="E47" s="63"/>
-      <c r="F47" s="63"/>
-      <c r="G47" s="63"/>
+      <c r="A47" s="69"/>
+      <c r="B47" s="69"/>
+      <c r="C47" s="69"/>
+      <c r="D47" s="69"/>
+      <c r="E47" s="69"/>
+      <c r="F47" s="69"/>
+      <c r="G47" s="69"/>
       <c r="AW47" s="0" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="63"/>
-      <c r="B48" s="63"/>
-      <c r="C48" s="63"/>
-      <c r="D48" s="63"/>
-      <c r="E48" s="63"/>
-      <c r="F48" s="63"/>
-      <c r="G48" s="63"/>
+      <c r="A48" s="69"/>
+      <c r="B48" s="69"/>
+      <c r="C48" s="69"/>
+      <c r="D48" s="69"/>
+      <c r="E48" s="69"/>
+      <c r="F48" s="69"/>
+      <c r="G48" s="69"/>
       <c r="AW48" s="0" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="63"/>
-      <c r="B49" s="63"/>
-      <c r="C49" s="63"/>
-      <c r="D49" s="63"/>
-      <c r="E49" s="63"/>
-      <c r="F49" s="63"/>
-      <c r="G49" s="63"/>
+      <c r="A49" s="69"/>
+      <c r="B49" s="69"/>
+      <c r="C49" s="69"/>
+      <c r="D49" s="69"/>
+      <c r="E49" s="69"/>
+      <c r="F49" s="69"/>
+      <c r="G49" s="69"/>
       <c r="AW49" s="0" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="63"/>
-      <c r="B50" s="63"/>
-      <c r="C50" s="63"/>
-      <c r="D50" s="63"/>
-      <c r="E50" s="63"/>
-      <c r="F50" s="63"/>
-      <c r="G50" s="63"/>
+      <c r="A50" s="69"/>
+      <c r="B50" s="69"/>
+      <c r="C50" s="69"/>
+      <c r="D50" s="69"/>
+      <c r="E50" s="69"/>
+      <c r="F50" s="69"/>
+      <c r="G50" s="69"/>
       <c r="AW50" s="0" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="63"/>
-      <c r="B51" s="63"/>
-      <c r="C51" s="63"/>
-      <c r="D51" s="63"/>
-      <c r="E51" s="63"/>
-      <c r="F51" s="63"/>
-      <c r="G51" s="63"/>
+      <c r="A51" s="69"/>
+      <c r="B51" s="69"/>
+      <c r="C51" s="69"/>
+      <c r="D51" s="69"/>
+      <c r="E51" s="69"/>
+      <c r="F51" s="69"/>
+      <c r="G51" s="69"/>
       <c r="AW51" s="0" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="63"/>
-      <c r="B52" s="63"/>
-      <c r="C52" s="63"/>
-      <c r="D52" s="63"/>
-      <c r="E52" s="63"/>
-      <c r="F52" s="63"/>
-      <c r="G52" s="63"/>
+      <c r="A52" s="69"/>
+      <c r="B52" s="69"/>
+      <c r="C52" s="69"/>
+      <c r="D52" s="69"/>
+      <c r="E52" s="69"/>
+      <c r="F52" s="69"/>
+      <c r="G52" s="69"/>
       <c r="AW52" s="0" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="63"/>
-      <c r="B53" s="63"/>
-      <c r="C53" s="63"/>
-      <c r="D53" s="63"/>
-      <c r="E53" s="63"/>
-      <c r="F53" s="63"/>
-      <c r="G53" s="63"/>
+      <c r="A53" s="69"/>
+      <c r="B53" s="69"/>
+      <c r="C53" s="69"/>
+      <c r="D53" s="69"/>
+      <c r="E53" s="69"/>
+      <c r="F53" s="69"/>
+      <c r="G53" s="69"/>
       <c r="AW53" s="0" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="63"/>
-      <c r="B54" s="63"/>
-      <c r="C54" s="63"/>
-      <c r="D54" s="63"/>
-      <c r="E54" s="63"/>
-      <c r="F54" s="63"/>
-      <c r="G54" s="63"/>
+      <c r="A54" s="69"/>
+      <c r="B54" s="69"/>
+      <c r="C54" s="69"/>
+      <c r="D54" s="69"/>
+      <c r="E54" s="69"/>
+      <c r="F54" s="69"/>
+      <c r="G54" s="69"/>
       <c r="AW54" s="0" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="63"/>
-      <c r="B55" s="63"/>
-      <c r="C55" s="63"/>
-      <c r="D55" s="63"/>
-      <c r="E55" s="63"/>
-      <c r="F55" s="63"/>
-      <c r="G55" s="63"/>
+      <c r="A55" s="69"/>
+      <c r="B55" s="69"/>
+      <c r="C55" s="69"/>
+      <c r="D55" s="69"/>
+      <c r="E55" s="69"/>
+      <c r="F55" s="69"/>
+      <c r="G55" s="69"/>
       <c r="AW55" s="0" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="63"/>
-      <c r="B56" s="63"/>
-      <c r="C56" s="63"/>
-      <c r="D56" s="63"/>
-      <c r="E56" s="63"/>
-      <c r="F56" s="63"/>
-      <c r="G56" s="63"/>
+      <c r="A56" s="69"/>
+      <c r="B56" s="69"/>
+      <c r="C56" s="69"/>
+      <c r="D56" s="69"/>
+      <c r="E56" s="69"/>
+      <c r="F56" s="69"/>
+      <c r="G56" s="69"/>
       <c r="AW56" s="0" t="s">
         <v>62</v>
       </c>

</xml_diff>